<commit_message>
avanzo para la 2da entrega
</commit_message>
<xml_diff>
--- a/preentregas/01ra_preentrega_tablas.xlsx
+++ b/preentregas/01ra_preentrega_tablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leeca\OneDrive\바탕 화면\Estudio\Coderhouse - SQL\Proyecto\preentregas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55AB17F-B28C-4D6A-A9AC-938B9C941217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C90F9F7-590D-4E82-BDBB-0C9C970F605B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -528,26 +528,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -728,6 +708,26 @@
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -742,17 +742,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01A6DE81-E2DF-4768-A1DF-66B854B5FADC}" name="Tabla1" displayName="Tabla1" ref="A3:H9" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01A6DE81-E2DF-4768-A1DF-66B854B5FADC}" name="Tabla1" displayName="Tabla1" ref="A3:H9" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A3:H9" xr:uid="{01A6DE81-E2DF-4768-A1DF-66B854B5FADC}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{2B806F74-40ED-483A-A551-34C757FB07EF}" name="Key" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{EEC88163-7FEA-4B52-8D45-C1A9ACD87D28}" name="Columna" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{550C58BF-67F7-427C-BCCA-AACAD30DEE56}" name="Tipo" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{A9D0FE59-D7AE-454F-9F3E-37E1E7791993}" name="Longitud" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{FDEE014B-E303-4163-B495-50387D5E3A62}" name="Not Null" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{E3E0F9A7-237C-419A-88CD-91620B439F32}" name="Único" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{DC22BFB2-0C81-47EB-B65D-99DA404051B3}" name="Default" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{E816D5C8-59E2-4366-B55C-241876A040C1}" name="Descripción" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{2B806F74-40ED-483A-A551-34C757FB07EF}" name="Key" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{EEC88163-7FEA-4B52-8D45-C1A9ACD87D28}" name="Columna" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{550C58BF-67F7-427C-BCCA-AACAD30DEE56}" name="Tipo" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{A9D0FE59-D7AE-454F-9F3E-37E1E7791993}" name="Longitud" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{FDEE014B-E303-4163-B495-50387D5E3A62}" name="Not Null" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{E3E0F9A7-237C-419A-88CD-91620B439F32}" name="Único" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{DC22BFB2-0C81-47EB-B65D-99DA404051B3}" name="Default" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{E816D5C8-59E2-4366-B55C-241876A040C1}" name="Descripción" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1210,18 +1210,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71:XFD71"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="A129" sqref="A129:H141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.75" customWidth="1"/>
-    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.375" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="8.625" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="7" max="7" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.375" customWidth="1"/>
+    <col min="7" max="7" width="11.75" customWidth="1"/>
+    <col min="8" max="8" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="21.75" x14ac:dyDescent="0.3">

</xml_diff>